<commit_message>
Example Fake_Data_1A added . bug in _q resolved
</commit_message>
<xml_diff>
--- a/parameters/Fake_Data_2/JCT_m_q.xlsx
+++ b/parameters/Fake_Data_2/JCT_m_q.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhsengland-my.sharepoint.com/personal/martina_fonseca_england_nhs_uk/Documents/Documents/Projects/AmbModelOpen/parameters/Fake_Data_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{2E949D65-BD68-46BF-B9F7-21ADE043105F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6A9A514-A584-4C08-8C45-EAAF53CABBEB}"/>
+  <xr:revisionPtr revIDLastSave="243" documentId="8_{2E949D65-BD68-46BF-B9F7-21ADE043105F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3579807-0687-4CD7-9EDB-3CAC5FEDFB59}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="traveltoscene" sheetId="1" r:id="rId1"/>
@@ -9979,15 +9979,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10031,7 +10031,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -10071,7 +10071,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -10191,7 +10191,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -10231,9 +10231,9 @@
         <v>71.3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0.01</v>
@@ -10255,7 +10255,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -10275,7 +10275,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -10295,7 +10295,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -10335,7 +10335,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -10355,7 +10355,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -10395,7 +10395,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -10415,7 +10415,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -10455,7 +10455,7 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -10467,7 +10467,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -10479,7 +10479,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -10491,7 +10491,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -10503,7 +10503,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -10515,7 +10515,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -10527,7 +10527,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -10539,7 +10539,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -10551,7 +10551,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -10563,7 +10563,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -10575,7 +10575,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -10604,15 +10604,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -10632,7 +10632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -10676,7 +10676,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -10696,7 +10696,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -10736,7 +10736,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>52.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -10776,7 +10776,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>62.3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -10836,7 +10836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -10856,9 +10856,9 @@
         <v>113.9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0.01</v>
@@ -10880,7 +10880,7 @@
         <v>2.7100000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -10920,7 +10920,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -10940,7 +10940,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -10980,7 +10980,7 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -11000,7 +11000,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -11020,7 +11020,7 @@
         <v>102.1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -11040,7 +11040,7 @@
         <v>111.8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -11060,7 +11060,7 @@
         <v>133.9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>137.1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -11092,7 +11092,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -11104,7 +11104,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -11116,7 +11116,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -11128,7 +11128,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -11140,7 +11140,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -11152,7 +11152,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -11164,7 +11164,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -11176,7 +11176,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -11188,7 +11188,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -11200,7 +11200,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -11229,15 +11229,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -11257,7 +11257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -11341,7 +11341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -11361,7 +11361,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -11421,7 +11421,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -11441,7 +11441,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -11481,9 +11481,9 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0.01</v>
@@ -11493,7 +11493,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -11517,7 +11517,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -11529,7 +11529,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -11541,7 +11541,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -11553,7 +11553,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -11565,7 +11565,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -11577,7 +11577,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -11589,7 +11589,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -11601,7 +11601,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -11613,7 +11613,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -11625,7 +11625,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -11637,7 +11637,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -11649,7 +11649,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -11661,7 +11661,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -11673,7 +11673,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -11685,7 +11685,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -11697,7 +11697,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -11709,7 +11709,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -11721,7 +11721,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -11733,7 +11733,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -11762,15 +11762,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -11790,7 +11790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11830,7 +11830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -11850,7 +11850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -11890,7 +11890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -11930,7 +11930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -11950,7 +11950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -11970,7 +11970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -11990,7 +11990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -12010,9 +12010,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0.01</v>
@@ -12022,7 +12022,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -12034,7 +12034,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -12046,7 +12046,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -12058,7 +12058,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -12070,7 +12070,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -12082,7 +12082,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -12094,7 +12094,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -12106,7 +12106,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -12118,7 +12118,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -12130,7 +12130,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -12142,7 +12142,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -12154,7 +12154,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -12166,7 +12166,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -12178,7 +12178,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -12190,7 +12190,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -12202,7 +12202,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -12214,7 +12214,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -12226,7 +12226,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -12238,7 +12238,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -12250,7 +12250,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -12262,7 +12262,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -12291,15 +12291,15 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -12343,7 +12343,7 @@
         <v>0.45999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -12363,7 +12363,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -12383,7 +12383,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -12423,7 +12423,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -12443,7 +12443,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -12463,7 +12463,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -12503,7 +12503,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -12523,7 +12523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -12543,9 +12543,9 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="2">
         <v>0.01</v>
@@ -12555,7 +12555,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -12567,7 +12567,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -12579,7 +12579,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -12591,7 +12591,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -12603,7 +12603,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -12615,7 +12615,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -12627,7 +12627,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -12639,7 +12639,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -12651,7 +12651,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -12663,7 +12663,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -12675,7 +12675,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3</v>
       </c>
@@ -12687,7 +12687,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -12699,7 +12699,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>3</v>
       </c>
@@ -12711,7 +12711,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -12723,7 +12723,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>3</v>
       </c>
@@ -12735,7 +12735,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -12747,7 +12747,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -12759,7 +12759,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>3</v>
       </c>
@@ -12771,7 +12771,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>3</v>
       </c>
@@ -12783,7 +12783,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -12795,7 +12795,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -12824,15 +12824,15 @@
   <dimension ref="A2:X110"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I103" sqref="I103"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -12860,23 +12860,23 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="4">
-        <f>SUMIF(C11:F110,"FALSE")</f>
+        <f>COUNTIF(C11:F110,"FALSE")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
@@ -12890,7 +12890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -12898,7 +12898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -12906,7 +12906,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -12930,7 +12930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -12978,7 +12978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -13002,7 +13002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -13050,7 +13050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -13098,7 +13098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -13123,7 +13123,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -13155,7 +13155,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -13227,7 +13227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -13251,7 +13251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -13275,7 +13275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -13299,7 +13299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -13323,7 +13323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -13347,7 +13347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -13395,12 +13395,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
@@ -13414,7 +13414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>1</v>
       </c>
@@ -13430,7 +13430,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>1</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>1</v>
       </c>
@@ -13478,7 +13478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>1</v>
       </c>
@@ -13502,7 +13502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -13526,7 +13526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>1</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>1</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -13598,7 +13598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -13622,7 +13622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>1</v>
       </c>
@@ -13670,7 +13670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>1</v>
       </c>
@@ -13678,7 +13678,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>2</v>
       </c>
@@ -13702,7 +13702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>2</v>
       </c>
@@ -13726,7 +13726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>2</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -13774,7 +13774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>2</v>
       </c>
@@ -13798,7 +13798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>2</v>
       </c>
@@ -13822,7 +13822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>2</v>
       </c>
@@ -13846,7 +13846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>2</v>
       </c>
@@ -13870,7 +13870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>2</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>2</v>
       </c>
@@ -13918,12 +13918,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C64" s="1" t="s">
         <v>0</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -13945,7 +13945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>1</v>
       </c>
@@ -13953,7 +13953,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>1</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -14001,7 +14001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>1</v>
       </c>
@@ -14025,7 +14025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>1</v>
       </c>
@@ -14049,7 +14049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>1</v>
       </c>
@@ -14073,7 +14073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>1</v>
       </c>
@@ -14097,7 +14097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>1</v>
       </c>
@@ -14121,7 +14121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -14145,7 +14145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>1</v>
       </c>
@@ -14169,7 +14169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>1</v>
       </c>
@@ -14193,12 +14193,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C81" s="1" t="s">
         <v>0</v>
       </c>
@@ -14212,7 +14212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>5</v>
       </c>
@@ -14220,7 +14220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>1</v>
       </c>
@@ -14228,7 +14228,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>1</v>
       </c>
@@ -14252,7 +14252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>1</v>
       </c>
@@ -14276,7 +14276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>1</v>
       </c>
@@ -14300,7 +14300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>1</v>
       </c>
@@ -14324,7 +14324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>1</v>
       </c>
@@ -14348,7 +14348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>1</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>1</v>
       </c>
@@ -14396,7 +14396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>1</v>
       </c>
@@ -14420,7 +14420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>1</v>
       </c>
@@ -14444,7 +14444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>1</v>
       </c>
@@ -14468,12 +14468,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C98" s="1" t="s">
         <v>0</v>
       </c>
@@ -14487,7 +14487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>5</v>
       </c>
@@ -14495,7 +14495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>1</v>
       </c>
@@ -14503,7 +14503,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>1</v>
       </c>
@@ -14527,7 +14527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>1</v>
       </c>
@@ -14551,7 +14551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -14575,7 +14575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>1</v>
       </c>
@@ -14599,7 +14599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>1</v>
       </c>
@@ -14623,7 +14623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>1</v>
       </c>
@@ -14647,7 +14647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>1</v>
       </c>
@@ -14671,7 +14671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>1</v>
       </c>
@@ -14695,7 +14695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>1</v>
       </c>
@@ -14719,7 +14719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>1</v>
       </c>

</xml_diff>